<commit_message>
Agregado timestamp en trama
</commit_message>
<xml_diff>
--- a/docs/Trama.xlsx
+++ b/docs/Trama.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Reportes" sheetId="3" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="129">
   <si>
     <t>Sensor</t>
   </si>
@@ -399,6 +399,21 @@
   </si>
   <si>
     <t>011e007b0631004d0052000a0078063400570052000e00770610006200520010007405e9006b0052000f</t>
+  </si>
+  <si>
+    <t>largo</t>
+  </si>
+  <si>
+    <t>Reporte #3</t>
+  </si>
+  <si>
+    <t>Timestamp [ultima]</t>
+  </si>
+  <si>
+    <t>uint32</t>
+  </si>
+  <si>
+    <t>seconds since UNIX epoch</t>
   </si>
 </sst>
 </file>
@@ -800,10 +815,10 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="4" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="4" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1170,10 +1185,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M39"/>
+  <dimension ref="A1:M69"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="C69" sqref="C69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1181,7 +1196,7 @@
     <col min="1" max="1" width="28.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.140625" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1660,8 +1675,375 @@
         <v>1</v>
       </c>
     </row>
+    <row r="42" spans="1:4">
+      <c r="A42" s="31" t="s">
+        <v>125</v>
+      </c>
+      <c r="B42" s="32"/>
+    </row>
+    <row r="43" spans="1:4">
+      <c r="A43" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B43" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
+      <c r="A44" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="B44" s="7">
+        <f>C69</f>
+        <v>45</v>
+      </c>
+      <c r="C44" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
+      <c r="A45" s="33" t="s">
+        <v>61</v>
+      </c>
+      <c r="B45" s="34"/>
+      <c r="C45" s="34"/>
+      <c r="D45" s="34"/>
+    </row>
+    <row r="46" spans="1:4">
+      <c r="A46" s="4" t="s">
+        <v>62</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="C46" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="D46" s="8" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
+      <c r="A47" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B47" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="C47" s="5">
+        <v>1</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
+      <c r="A48" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>127</v>
+      </c>
+      <c r="C48" s="5">
+        <v>4</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
+      <c r="A49" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C49" s="5">
+        <v>2</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
+      <c r="A50" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C50" s="5">
+        <v>2</v>
+      </c>
+      <c r="D50" s="9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
+      <c r="A51" s="5" t="s">
+        <v>85</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="C51" s="5">
+        <v>2</v>
+      </c>
+      <c r="D51" s="10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4">
+      <c r="A52" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="B52" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C52" s="5">
+        <v>2</v>
+      </c>
+      <c r="D52" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="53" spans="1:4">
+      <c r="A53" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="B53" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C53" s="5">
+        <v>2</v>
+      </c>
+      <c r="D53" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="54" spans="1:4">
+      <c r="A54" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="B54" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C54" s="5">
+        <v>2</v>
+      </c>
+      <c r="D54" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="55" spans="1:4">
+      <c r="A55" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B55" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C55" s="5">
+        <v>2</v>
+      </c>
+      <c r="D55" s="9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="56" spans="1:4">
+      <c r="A56" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="C56" s="5">
+        <v>2</v>
+      </c>
+      <c r="D56" s="10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="57" spans="1:4">
+      <c r="A57" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C57" s="5">
+        <v>2</v>
+      </c>
+      <c r="D57" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="58" spans="1:4">
+      <c r="A58" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C58" s="5">
+        <v>2</v>
+      </c>
+      <c r="D58" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="59" spans="1:4">
+      <c r="A59" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C59" s="5">
+        <v>2</v>
+      </c>
+      <c r="D59" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="60" spans="1:4">
+      <c r="A60" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C60" s="5">
+        <v>2</v>
+      </c>
+      <c r="D60" s="9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4">
+      <c r="A61" s="5" t="s">
+        <v>100</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="C61" s="5">
+        <v>2</v>
+      </c>
+      <c r="D61" s="10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4">
+      <c r="A62" s="5" t="s">
+        <v>101</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C62" s="5">
+        <v>2</v>
+      </c>
+      <c r="D62" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4">
+      <c r="A63" s="5" t="s">
+        <v>102</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C63" s="5">
+        <v>2</v>
+      </c>
+      <c r="D63" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4">
+      <c r="A64" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C64" s="5">
+        <v>2</v>
+      </c>
+      <c r="D64" s="5" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="65" spans="1:4">
+      <c r="A65" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C65" s="5">
+        <v>2</v>
+      </c>
+      <c r="D65" s="9" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="66" spans="1:4">
+      <c r="A66" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="C66" s="5">
+        <v>2</v>
+      </c>
+      <c r="D66" s="10" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="67" spans="1:4">
+      <c r="A67" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C67" s="5">
+        <v>2</v>
+      </c>
+      <c r="D67" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4">
+      <c r="A68" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>97</v>
+      </c>
+      <c r="C68" s="5">
+        <v>2</v>
+      </c>
+      <c r="D68" s="5" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4">
+      <c r="B69" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="C69" s="11">
+        <f>SUM(C47:C68)</f>
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="5">
+  <mergeCells count="7">
+    <mergeCell ref="A42:B42"/>
+    <mergeCell ref="A45:D45"/>
     <mergeCell ref="A33:B33"/>
     <mergeCell ref="A36:D36"/>
     <mergeCell ref="A5:B5"/>
@@ -1676,8 +2058,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1690,15 +2072,24 @@
       <c r="A1" s="12" t="s">
         <v>113</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="37" t="s">
         <v>123</v>
       </c>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="37"/>
-      <c r="F1" s="37"/>
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
       <c r="G1" t="s">
         <v>119</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>124</v>
+      </c>
+      <c r="B2">
+        <f>LEN(B1)/2</f>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" thickBot="1"/>
@@ -2147,7 +2538,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
Restaurado ComRS232 y Quitado multiplicador de turbidez
</commit_message>
<xml_diff>
--- a/docs/Trama.xlsx
+++ b/docs/Trama.xlsx
@@ -1,33 +1,42 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24701"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Emir Promatix\Dropbox\TAREAS\secretaria\est_monit_rio_jachal\Software Datalogger\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\ProMatix\Dropbox\TAREAS\secretaria\est_monit_rio_jachal\Software Datalogger\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7B62516-D7E0-423C-A733-F52F6590B761}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Reportes" sheetId="3" r:id="rId1"/>
-    <sheet name="Decodificador" sheetId="4" r:id="rId2"/>
-    <sheet name="Variables" sheetId="1" r:id="rId3"/>
-    <sheet name="Tablas" sheetId="2" r:id="rId4"/>
+    <sheet name="Decodificador ID 01" sheetId="4" r:id="rId2"/>
+    <sheet name="Decodificador ID 03" sheetId="5" r:id="rId3"/>
+    <sheet name="Variables" sheetId="1" r:id="rId4"/>
+    <sheet name="Tablas" sheetId="2" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="129">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="422" uniqueCount="135">
   <si>
     <t>Sensor</t>
   </si>
@@ -398,9 +407,6 @@
     <t>PH</t>
   </si>
   <si>
-    <t>011e007b0631004d0052000a0078063400570052000e00770610006200520010007405e9006b0052000f</t>
-  </si>
-  <si>
     <t>largo</t>
   </si>
   <si>
@@ -413,13 +419,34 @@
     <t>uint32</t>
   </si>
   <si>
-    <t>seconds since UNIX epoch</t>
+    <t>031461c3233011111221133114411551211222222332244225523113322333333443355341144224433444444554</t>
+  </si>
+  <si>
+    <t>largo [bytes]</t>
+  </si>
+  <si>
+    <t>Posicion</t>
+  </si>
+  <si>
+    <t>UTC</t>
+  </si>
+  <si>
+    <t>Seg</t>
+  </si>
+  <si>
+    <t>031461c3053011111221133114411551211222222332244225523113322333333443355341144224433444444554</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FBU </t>
+  </si>
+  <si>
+    <t>segundos desde UNIX epoch (UTC)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="4">
     <font>
       <sz val="11"/>
@@ -484,7 +511,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="28">
     <border>
       <left/>
       <right/>
@@ -732,6 +759,113 @@
         <color indexed="64"/>
       </top>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -743,7 +877,7 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="72">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -816,11 +950,54 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="5" xfId="4" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="4" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="19" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="20" xfId="5" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="21" xfId="5" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="20" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="2" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="21" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="5" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="22" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="23" xfId="4" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="5" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="9" xfId="5" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="12" xfId="5" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="2" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="24" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="6">
     <cellStyle name="20% - Énfasis1" xfId="4" builtinId="30"/>
@@ -860,29 +1037,29 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tabla1" displayName="Tabla1" ref="A1:H13" totalsRowShown="0">
-  <autoFilter ref="A1:H13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Tabla1" displayName="Tabla1" ref="A1:H13" totalsRowShown="0">
+  <autoFilter ref="A1:H13" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="8">
-    <tableColumn id="1" name="Varible"/>
-    <tableColumn id="2" name="Tipo"/>
-    <tableColumn id="5" name="Unidad"/>
-    <tableColumn id="3" name="Sensor"/>
-    <tableColumn id="4" name="Descripcion"/>
-    <tableColumn id="6" name="Nota"/>
-    <tableColumn id="7" name="Transmite"/>
-    <tableColumn id="8" name="Rango tipico"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Varible"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Tipo"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Unidad"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Sensor"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Descripcion"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="Nota"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="Transmite"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0000-000008000000}" name="Rango tipico"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Tabla2" displayName="Tabla2" ref="A1:C3" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
-  <autoFilter ref="A1:C3"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{00000000-000C-0000-FFFF-FFFF01000000}" name="Tabla2" displayName="Tabla2" ref="A1:C3" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+  <autoFilter ref="A1:C3" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Tabla" dataDxfId="2"/>
-    <tableColumn id="3" name="Intervalo" dataDxfId="1"/>
-    <tableColumn id="4" name="Variables" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0100-000001000000}" name="Tabla" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0100-000003000000}" name="Intervalo" dataDxfId="1"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0100-000004000000}" name="Variables" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium21" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1184,11 +1361,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M69"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="C69" sqref="C69"/>
+      <selection activeCell="G61" sqref="G61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -1196,7 +1373,7 @@
     <col min="1" max="1" width="28.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.85546875" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="11.7109375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1677,7 +1854,7 @@
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="31" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B42" s="32"/>
     </row>
@@ -1709,64 +1886,64 @@
       <c r="C45" s="34"/>
       <c r="D45" s="34"/>
     </row>
-    <row r="46" spans="1:4">
-      <c r="A46" s="4" t="s">
+    <row r="46" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A46" s="6" t="s">
         <v>62</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="B46" s="6" t="s">
         <v>63</v>
       </c>
-      <c r="C46" s="8" t="s">
+      <c r="C46" s="60" t="s">
         <v>89</v>
       </c>
-      <c r="D46" s="8" t="s">
+      <c r="D46" s="60" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="47" spans="1:4">
-      <c r="A47" s="5" t="s">
+      <c r="A47" s="61" t="s">
         <v>82</v>
       </c>
-      <c r="B47" s="5" t="s">
+      <c r="B47" s="62" t="s">
         <v>96</v>
       </c>
-      <c r="C47" s="5">
+      <c r="C47" s="62">
         <v>1</v>
       </c>
-      <c r="D47" s="5" t="s">
+      <c r="D47" s="63" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="48" spans="1:4">
-      <c r="A48" s="5" t="s">
+    <row r="48" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A48" s="64" t="s">
+        <v>125</v>
+      </c>
+      <c r="B48" s="65" t="s">
         <v>126</v>
       </c>
-      <c r="B48" s="5" t="s">
-        <v>127</v>
-      </c>
-      <c r="C48" s="5">
+      <c r="C48" s="65">
         <v>4</v>
       </c>
-      <c r="D48" s="5" t="s">
-        <v>128</v>
+      <c r="D48" s="66" t="s">
+        <v>134</v>
       </c>
     </row>
     <row r="49" spans="1:4">
-      <c r="A49" s="5" t="s">
+      <c r="A49" s="61" t="s">
         <v>83</v>
       </c>
-      <c r="B49" s="5" t="s">
+      <c r="B49" s="62" t="s">
         <v>97</v>
       </c>
-      <c r="C49" s="5">
-        <v>2</v>
-      </c>
-      <c r="D49" s="5" t="s">
+      <c r="C49" s="62">
+        <v>2</v>
+      </c>
+      <c r="D49" s="63" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="50" spans="1:4">
-      <c r="A50" s="5" t="s">
+      <c r="A50" s="67" t="s">
         <v>84</v>
       </c>
       <c r="B50" s="5" t="s">
@@ -1775,12 +1952,12 @@
       <c r="C50" s="5">
         <v>2</v>
       </c>
-      <c r="D50" s="9" t="s">
+      <c r="D50" s="68" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="51" spans="1:4">
-      <c r="A51" s="5" t="s">
+      <c r="A51" s="67" t="s">
         <v>85</v>
       </c>
       <c r="B51" s="5" t="s">
@@ -1789,12 +1966,12 @@
       <c r="C51" s="5">
         <v>2</v>
       </c>
-      <c r="D51" s="10" t="s">
+      <c r="D51" s="69" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="52" spans="1:4">
-      <c r="A52" s="5" t="s">
+      <c r="A52" s="67" t="s">
         <v>86</v>
       </c>
       <c r="B52" s="5" t="s">
@@ -1803,40 +1980,40 @@
       <c r="C52" s="5">
         <v>2</v>
       </c>
-      <c r="D52" s="10" t="s">
+      <c r="D52" s="69" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="53" spans="1:4">
-      <c r="A53" s="5" t="s">
+    <row r="53" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A53" s="64" t="s">
         <v>87</v>
       </c>
-      <c r="B53" s="5" t="s">
+      <c r="B53" s="65" t="s">
         <v>97</v>
       </c>
-      <c r="C53" s="5">
-        <v>2</v>
-      </c>
-      <c r="D53" s="5" t="s">
-        <v>76</v>
+      <c r="C53" s="65">
+        <v>2</v>
+      </c>
+      <c r="D53" s="66" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="54" spans="1:4">
-      <c r="A54" s="5" t="s">
+      <c r="A54" s="61" t="s">
         <v>91</v>
       </c>
-      <c r="B54" s="5" t="s">
+      <c r="B54" s="62" t="s">
         <v>97</v>
       </c>
-      <c r="C54" s="5">
-        <v>2</v>
-      </c>
-      <c r="D54" s="5" t="s">
+      <c r="C54" s="62">
+        <v>2</v>
+      </c>
+      <c r="D54" s="63" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="55" spans="1:4">
-      <c r="A55" s="5" t="s">
+      <c r="A55" s="67" t="s">
         <v>92</v>
       </c>
       <c r="B55" s="5" t="s">
@@ -1845,12 +2022,12 @@
       <c r="C55" s="5">
         <v>2</v>
       </c>
-      <c r="D55" s="9" t="s">
+      <c r="D55" s="68" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="56" spans="1:4">
-      <c r="A56" s="5" t="s">
+      <c r="A56" s="67" t="s">
         <v>93</v>
       </c>
       <c r="B56" s="5" t="s">
@@ -1859,12 +2036,12 @@
       <c r="C56" s="5">
         <v>2</v>
       </c>
-      <c r="D56" s="10" t="s">
+      <c r="D56" s="69" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="57" spans="1:4">
-      <c r="A57" s="5" t="s">
+      <c r="A57" s="67" t="s">
         <v>94</v>
       </c>
       <c r="B57" s="5" t="s">
@@ -1873,40 +2050,40 @@
       <c r="C57" s="5">
         <v>2</v>
       </c>
-      <c r="D57" s="10" t="s">
+      <c r="D57" s="69" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="58" spans="1:4">
-      <c r="A58" s="5" t="s">
+    <row r="58" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A58" s="64" t="s">
         <v>95</v>
       </c>
-      <c r="B58" s="5" t="s">
+      <c r="B58" s="65" t="s">
         <v>97</v>
       </c>
-      <c r="C58" s="5">
-        <v>2</v>
-      </c>
-      <c r="D58" s="5" t="s">
-        <v>76</v>
+      <c r="C58" s="65">
+        <v>2</v>
+      </c>
+      <c r="D58" s="66" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="59" spans="1:4">
-      <c r="A59" s="5" t="s">
+      <c r="A59" s="61" t="s">
         <v>98</v>
       </c>
-      <c r="B59" s="5" t="s">
+      <c r="B59" s="62" t="s">
         <v>97</v>
       </c>
-      <c r="C59" s="5">
-        <v>2</v>
-      </c>
-      <c r="D59" s="5" t="s">
+      <c r="C59" s="62">
+        <v>2</v>
+      </c>
+      <c r="D59" s="63" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="60" spans="1:4">
-      <c r="A60" s="5" t="s">
+      <c r="A60" s="67" t="s">
         <v>99</v>
       </c>
       <c r="B60" s="5" t="s">
@@ -1915,12 +2092,12 @@
       <c r="C60" s="5">
         <v>2</v>
       </c>
-      <c r="D60" s="9" t="s">
+      <c r="D60" s="68" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="61" spans="1:4">
-      <c r="A61" s="5" t="s">
+      <c r="A61" s="67" t="s">
         <v>100</v>
       </c>
       <c r="B61" s="5" t="s">
@@ -1929,12 +2106,12 @@
       <c r="C61" s="5">
         <v>2</v>
       </c>
-      <c r="D61" s="10" t="s">
+      <c r="D61" s="69" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="62" spans="1:4">
-      <c r="A62" s="5" t="s">
+      <c r="A62" s="67" t="s">
         <v>101</v>
       </c>
       <c r="B62" s="5" t="s">
@@ -1943,40 +2120,40 @@
       <c r="C62" s="5">
         <v>2</v>
       </c>
-      <c r="D62" s="10" t="s">
+      <c r="D62" s="69" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="63" spans="1:4">
-      <c r="A63" s="5" t="s">
+    <row r="63" spans="1:4" ht="15.75" thickBot="1">
+      <c r="A63" s="64" t="s">
         <v>102</v>
       </c>
-      <c r="B63" s="5" t="s">
+      <c r="B63" s="65" t="s">
         <v>97</v>
       </c>
-      <c r="C63" s="5">
-        <v>2</v>
-      </c>
-      <c r="D63" s="5" t="s">
-        <v>76</v>
+      <c r="C63" s="65">
+        <v>2</v>
+      </c>
+      <c r="D63" s="66" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="64" spans="1:4">
-      <c r="A64" s="5" t="s">
+      <c r="A64" s="61" t="s">
         <v>103</v>
       </c>
-      <c r="B64" s="5" t="s">
+      <c r="B64" s="62" t="s">
         <v>97</v>
       </c>
-      <c r="C64" s="5">
-        <v>2</v>
-      </c>
-      <c r="D64" s="5" t="s">
+      <c r="C64" s="62">
+        <v>2</v>
+      </c>
+      <c r="D64" s="63" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="65" spans="1:4">
-      <c r="A65" s="5" t="s">
+    <row r="65" spans="1:5">
+      <c r="A65" s="67" t="s">
         <v>104</v>
       </c>
       <c r="B65" s="5" t="s">
@@ -1985,12 +2162,12 @@
       <c r="C65" s="5">
         <v>2</v>
       </c>
-      <c r="D65" s="9" t="s">
+      <c r="D65" s="68" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="66" spans="1:4">
-      <c r="A66" s="5" t="s">
+    <row r="66" spans="1:5">
+      <c r="A66" s="67" t="s">
         <v>105</v>
       </c>
       <c r="B66" s="5" t="s">
@@ -1999,12 +2176,12 @@
       <c r="C66" s="5">
         <v>2</v>
       </c>
-      <c r="D66" s="10" t="s">
+      <c r="D66" s="69" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="67" spans="1:4">
-      <c r="A67" s="5" t="s">
+    <row r="67" spans="1:5">
+      <c r="A67" s="67" t="s">
         <v>106</v>
       </c>
       <c r="B67" s="5" t="s">
@@ -2013,59 +2190,62 @@
       <c r="C67" s="5">
         <v>2</v>
       </c>
-      <c r="D67" s="10" t="s">
+      <c r="D67" s="69" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="68" spans="1:4">
-      <c r="A68" s="5" t="s">
+      <c r="E67" s="59"/>
+    </row>
+    <row r="68" spans="1:5" ht="15.75" thickBot="1">
+      <c r="A68" s="64" t="s">
         <v>107</v>
       </c>
-      <c r="B68" s="5" t="s">
+      <c r="B68" s="65" t="s">
         <v>97</v>
       </c>
-      <c r="C68" s="5">
-        <v>2</v>
-      </c>
-      <c r="D68" s="5" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4">
-      <c r="B69" s="4" t="s">
+      <c r="C68" s="65">
+        <v>2</v>
+      </c>
+      <c r="D68" s="66" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5">
+      <c r="B69" s="70" t="s">
         <v>88</v>
       </c>
-      <c r="C69" s="11">
+      <c r="C69" s="71">
         <f>SUM(C47:C68)</f>
         <v>45</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="H1:M1"/>
     <mergeCell ref="A42:B42"/>
     <mergeCell ref="A45:D45"/>
     <mergeCell ref="A33:B33"/>
     <mergeCell ref="A36:D36"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="A8:D8"/>
-    <mergeCell ref="H1:M1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="27" customWidth="1"/>
-    <col min="2" max="6" width="22.7109375" customWidth="1"/>
+    <col min="2" max="3" width="22.7109375" customWidth="1"/>
+    <col min="4" max="4" width="10.42578125" customWidth="1"/>
+    <col min="5" max="6" width="22.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7">
@@ -2073,7 +2253,7 @@
         <v>113</v>
       </c>
       <c r="B1" s="37" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="C1" s="38"/>
       <c r="D1" s="38"/>
@@ -2085,11 +2265,11 @@
     </row>
     <row r="2" spans="1:7">
       <c r="A2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B2">
         <f>LEN(B1)/2</f>
-        <v>42</v>
+        <v>46</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" thickBot="1"/>
@@ -2114,7 +2294,7 @@
       </c>
       <c r="B5" s="22" t="str">
         <f>MID($B$1,1,2)</f>
-        <v>01</v>
+        <v>03</v>
       </c>
       <c r="C5" s="23" t="s">
         <v>118</v>
@@ -2132,11 +2312,11 @@
       </c>
       <c r="B6" s="25" t="str">
         <f>MID($B$1,3,2)</f>
-        <v>1e</v>
+        <v>14</v>
       </c>
       <c r="C6" s="25">
         <f>(HEX2DEC(B6)/10)+10</f>
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D6" s="25" t="s">
         <v>120</v>
@@ -2151,11 +2331,11 @@
       </c>
       <c r="B7" s="22" t="str">
         <f>MID($B$1,5,4)</f>
-        <v>007b</v>
+        <v>61c3</v>
       </c>
       <c r="C7" s="22">
         <f>HEX2DEC(B7)/10</f>
-        <v>12.3</v>
+        <v>2502.6999999999998</v>
       </c>
       <c r="D7" s="22" t="s">
         <v>14</v>
@@ -2170,11 +2350,11 @@
       </c>
       <c r="B8" s="28" t="str">
         <f>MID($B$1,9,4)</f>
-        <v>0631</v>
+        <v>2330</v>
       </c>
       <c r="C8" s="28">
         <f>HEX2DEC(B8)/1000</f>
-        <v>1.585</v>
+        <v>9.0079999999999991</v>
       </c>
       <c r="D8" s="28" t="s">
         <v>21</v>
@@ -2189,11 +2369,11 @@
       </c>
       <c r="B9" s="28" t="str">
         <f>MID($B$1,13,4)</f>
-        <v>004d</v>
+        <v>1111</v>
       </c>
       <c r="C9" s="28">
         <f>HEX2DEC(B9)/10</f>
-        <v>7.7</v>
+        <v>436.9</v>
       </c>
       <c r="D9" s="28" t="s">
         <v>121</v>
@@ -2208,11 +2388,11 @@
       </c>
       <c r="B10" s="28" t="str">
         <f>MID($B$1,17,4)</f>
-        <v>0052</v>
+        <v>1221</v>
       </c>
       <c r="C10" s="28">
         <f>HEX2DEC(B10)/10</f>
-        <v>8.1999999999999993</v>
+        <v>464.1</v>
       </c>
       <c r="D10" s="28" t="s">
         <v>122</v>
@@ -2227,11 +2407,11 @@
       </c>
       <c r="B11" s="25" t="str">
         <f>MID($B$1,21,4)</f>
-        <v>000a</v>
+        <v>1331</v>
       </c>
       <c r="C11" s="25">
         <f>HEX2DEC(B11)*10</f>
-        <v>100</v>
+        <v>49130</v>
       </c>
       <c r="D11" s="25" t="s">
         <v>27</v>
@@ -2246,11 +2426,11 @@
       </c>
       <c r="B12" s="22" t="str">
         <f>MID($B$1,25,4)</f>
-        <v>0078</v>
+        <v>1441</v>
       </c>
       <c r="C12" s="22">
         <f t="shared" ref="C12" si="0">HEX2DEC(B12)/10</f>
-        <v>12</v>
+        <v>518.5</v>
       </c>
       <c r="D12" s="22" t="s">
         <v>14</v>
@@ -2265,11 +2445,11 @@
       </c>
       <c r="B13" s="28" t="str">
         <f>MID($B$1,29,4)</f>
-        <v>0634</v>
+        <v>1551</v>
       </c>
       <c r="C13" s="28">
         <f t="shared" ref="C13" si="1">HEX2DEC(B13)/1000</f>
-        <v>1.5880000000000001</v>
+        <v>5.4569999999999999</v>
       </c>
       <c r="D13" s="28" t="s">
         <v>21</v>
@@ -2284,11 +2464,11 @@
       </c>
       <c r="B14" s="28" t="str">
         <f>MID($B$1,33,4)</f>
-        <v>0057</v>
+        <v>2112</v>
       </c>
       <c r="C14" s="28">
         <f t="shared" ref="C14:C15" si="2">HEX2DEC(B14)/10</f>
-        <v>8.6999999999999993</v>
+        <v>846.6</v>
       </c>
       <c r="D14" s="28" t="s">
         <v>121</v>
@@ -2303,11 +2483,11 @@
       </c>
       <c r="B15" s="28" t="str">
         <f>MID($B$1,37,4)</f>
-        <v>0052</v>
+        <v>2222</v>
       </c>
       <c r="C15" s="28">
         <f t="shared" si="2"/>
-        <v>8.1999999999999993</v>
+        <v>873.8</v>
       </c>
       <c r="D15" s="28" t="s">
         <v>122</v>
@@ -2322,11 +2502,11 @@
       </c>
       <c r="B16" s="25" t="str">
         <f>MID($B$1,41,4)</f>
-        <v>000e</v>
+        <v>2332</v>
       </c>
       <c r="C16" s="25">
         <f t="shared" ref="C16" si="3">HEX2DEC(B16)*10</f>
-        <v>140</v>
+        <v>90100</v>
       </c>
       <c r="D16" s="25" t="s">
         <v>27</v>
@@ -2341,11 +2521,11 @@
       </c>
       <c r="B17" s="22" t="str">
         <f>MID($B$1,45,4)</f>
-        <v>0077</v>
+        <v>2442</v>
       </c>
       <c r="C17" s="22">
         <f t="shared" ref="C17" si="4">HEX2DEC(B17)/10</f>
-        <v>11.9</v>
+        <v>928.2</v>
       </c>
       <c r="D17" s="22" t="s">
         <v>14</v>
@@ -2360,11 +2540,11 @@
       </c>
       <c r="B18" s="28" t="str">
         <f>MID($B$1,49,4)</f>
-        <v>0610</v>
+        <v>2552</v>
       </c>
       <c r="C18" s="28">
         <f t="shared" ref="C18" si="5">HEX2DEC(B18)/1000</f>
-        <v>1.552</v>
+        <v>9.5540000000000003</v>
       </c>
       <c r="D18" s="28" t="s">
         <v>21</v>
@@ -2379,11 +2559,11 @@
       </c>
       <c r="B19" s="28" t="str">
         <f>MID($B$1,53,4)</f>
-        <v>0062</v>
+        <v>3113</v>
       </c>
       <c r="C19" s="28">
         <f t="shared" ref="C19:C20" si="6">HEX2DEC(B19)/10</f>
-        <v>9.8000000000000007</v>
+        <v>1256.3</v>
       </c>
       <c r="D19" s="28" t="s">
         <v>121</v>
@@ -2398,11 +2578,11 @@
       </c>
       <c r="B20" s="28" t="str">
         <f>MID($B$1,57,4)</f>
-        <v>0052</v>
+        <v>3223</v>
       </c>
       <c r="C20" s="28">
         <f t="shared" si="6"/>
-        <v>8.1999999999999993</v>
+        <v>1283.5</v>
       </c>
       <c r="D20" s="28" t="s">
         <v>122</v>
@@ -2417,11 +2597,11 @@
       </c>
       <c r="B21" s="25" t="str">
         <f>MID($B$1,61,4)</f>
-        <v>0010</v>
+        <v>3333</v>
       </c>
       <c r="C21" s="25">
         <f t="shared" ref="C21" si="7">HEX2DEC(B21)*10</f>
-        <v>160</v>
+        <v>131070</v>
       </c>
       <c r="D21" s="25" t="s">
         <v>27</v>
@@ -2436,11 +2616,11 @@
       </c>
       <c r="B22" s="22" t="str">
         <f>MID($B$1,65,4)</f>
-        <v>0074</v>
+        <v>3443</v>
       </c>
       <c r="C22" s="22">
         <f t="shared" ref="C22" si="8">HEX2DEC(B22)/10</f>
-        <v>11.6</v>
+        <v>1337.9</v>
       </c>
       <c r="D22" s="22" t="s">
         <v>14</v>
@@ -2455,11 +2635,11 @@
       </c>
       <c r="B23" s="28" t="str">
         <f>MID($B$1,69,4)</f>
-        <v>05e9</v>
+        <v>3553</v>
       </c>
       <c r="C23" s="28">
         <f t="shared" ref="C23" si="9">HEX2DEC(B23)/1000</f>
-        <v>1.5129999999999999</v>
+        <v>13.651</v>
       </c>
       <c r="D23" s="28" t="s">
         <v>21</v>
@@ -2474,11 +2654,11 @@
       </c>
       <c r="B24" s="28" t="str">
         <f>MID($B$1,73,4)</f>
-        <v>006b</v>
+        <v>4114</v>
       </c>
       <c r="C24" s="28">
         <f t="shared" ref="C24:C25" si="10">HEX2DEC(B24)/10</f>
-        <v>10.7</v>
+        <v>1666</v>
       </c>
       <c r="D24" s="28" t="s">
         <v>121</v>
@@ -2493,11 +2673,11 @@
       </c>
       <c r="B25" s="28" t="str">
         <f>MID($B$1,77,4)</f>
-        <v>0052</v>
+        <v>4224</v>
       </c>
       <c r="C25" s="28">
         <f t="shared" si="10"/>
-        <v>8.1999999999999993</v>
+        <v>1693.2</v>
       </c>
       <c r="D25" s="28" t="s">
         <v>122</v>
@@ -2512,11 +2692,11 @@
       </c>
       <c r="B26" s="25" t="str">
         <f>MID($B$1,81,4)</f>
-        <v>000f</v>
+        <v>4334</v>
       </c>
       <c r="C26" s="25">
         <f t="shared" ref="C26" si="11">HEX2DEC(B26)*10</f>
-        <v>150</v>
+        <v>172040</v>
       </c>
       <c r="D26" s="25" t="s">
         <v>27</v>
@@ -2534,7 +2714,685 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B8ABDE8-E1B6-48E7-9A10-E5E726EB722B}">
+  <dimension ref="A1:I27"/>
+  <sheetViews>
+    <sheetView topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G23" sqref="G23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <cols>
+    <col min="1" max="1" width="27" customWidth="1"/>
+    <col min="2" max="2" width="8.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.28515625" customWidth="1"/>
+    <col min="5" max="5" width="18.85546875" customWidth="1"/>
+    <col min="6" max="6" width="10.42578125" customWidth="1"/>
+    <col min="7" max="7" width="22.7109375" customWidth="1"/>
+    <col min="8" max="8" width="16.85546875" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9">
+      <c r="A1" s="12" t="s">
+        <v>113</v>
+      </c>
+      <c r="B1" s="39"/>
+      <c r="C1" s="39"/>
+      <c r="D1" s="37" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1" s="38"/>
+      <c r="F1" s="38"/>
+      <c r="G1" s="38"/>
+      <c r="H1" s="38"/>
+      <c r="I1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9">
+      <c r="A2" t="s">
+        <v>123</v>
+      </c>
+      <c r="D2">
+        <f>LEN(D1)/2</f>
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="15.75" thickBot="1"/>
+    <row r="4" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A4" s="19"/>
+      <c r="B4" s="40" t="s">
+        <v>129</v>
+      </c>
+      <c r="C4" s="40" t="s">
+        <v>128</v>
+      </c>
+      <c r="D4" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="E4" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="F4" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" s="21" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9">
+      <c r="A5" s="13" t="s">
+        <v>114</v>
+      </c>
+      <c r="B5" s="52">
+        <v>1</v>
+      </c>
+      <c r="C5" s="52">
+        <v>1</v>
+      </c>
+      <c r="D5" s="22" t="str">
+        <f>MID($D$1,(B5-1)*2+1,C5*2)</f>
+        <v>03</v>
+      </c>
+      <c r="E5" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="F5" s="23" t="s">
+        <v>118</v>
+      </c>
+      <c r="G5" s="24" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9">
+      <c r="A6" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="B6" s="51">
+        <f>B5+C5</f>
+        <v>2</v>
+      </c>
+      <c r="C6" s="51">
+        <v>1</v>
+      </c>
+      <c r="D6" s="28" t="str">
+        <f>MID($D$1,(B6-1)*2+1,C6*2)</f>
+        <v>14</v>
+      </c>
+      <c r="E6" s="28">
+        <f>(HEX2DEC(D6)/10)+10</f>
+        <v>12</v>
+      </c>
+      <c r="F6" s="28" t="s">
+        <v>120</v>
+      </c>
+      <c r="G6" s="53" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A7" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="B7" s="54">
+        <f t="shared" ref="B7:B27" si="0">B6+C6</f>
+        <v>3</v>
+      </c>
+      <c r="C7" s="54">
+        <v>4</v>
+      </c>
+      <c r="D7" s="25" t="str">
+        <f>MID($D$1,(B7-1)*2+1,C7*2)</f>
+        <v>61c30530</v>
+      </c>
+      <c r="E7" s="55">
+        <f>HEX2DEC(D7)</f>
+        <v>1640170800</v>
+      </c>
+      <c r="F7" s="25" t="s">
+        <v>131</v>
+      </c>
+      <c r="G7" s="56"/>
+      <c r="H7" s="57">
+        <f>(E7)/86400 + DATE(1970,1,1)</f>
+        <v>44552.458333333328</v>
+      </c>
+      <c r="I7" s="28" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9">
+      <c r="A8" s="47" t="s">
+        <v>83</v>
+      </c>
+      <c r="B8" s="48">
+        <f t="shared" si="0"/>
+        <v>7</v>
+      </c>
+      <c r="C8" s="48">
+        <v>2</v>
+      </c>
+      <c r="D8" s="49" t="str">
+        <f t="shared" ref="D8:D27" si="1">MID($D$1,(B8-1)*2+1,C8*2)</f>
+        <v>1111</v>
+      </c>
+      <c r="E8" s="49">
+        <f>HEX2DEC(D8)/10</f>
+        <v>436.9</v>
+      </c>
+      <c r="F8" s="49" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="50" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9">
+      <c r="A9" s="16" t="s">
+        <v>84</v>
+      </c>
+      <c r="B9" s="44">
+        <f t="shared" si="0"/>
+        <v>9</v>
+      </c>
+      <c r="C9" s="44">
+        <v>2</v>
+      </c>
+      <c r="D9" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v>1221</v>
+      </c>
+      <c r="E9" s="28">
+        <f>HEX2DEC(D9)/1000</f>
+        <v>4.641</v>
+      </c>
+      <c r="F9" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9" s="29" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9">
+      <c r="A10" s="16" t="s">
+        <v>85</v>
+      </c>
+      <c r="B10" s="44">
+        <f t="shared" si="0"/>
+        <v>11</v>
+      </c>
+      <c r="C10" s="44">
+        <v>2</v>
+      </c>
+      <c r="D10" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v>1331</v>
+      </c>
+      <c r="E10" s="28">
+        <f>HEX2DEC(D10)/10</f>
+        <v>491.3</v>
+      </c>
+      <c r="F10" s="28" t="s">
+        <v>121</v>
+      </c>
+      <c r="G10" s="30" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9">
+      <c r="A11" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="B11" s="44">
+        <f t="shared" si="0"/>
+        <v>13</v>
+      </c>
+      <c r="C11" s="44">
+        <v>2</v>
+      </c>
+      <c r="D11" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v>1441</v>
+      </c>
+      <c r="E11" s="28">
+        <f>HEX2DEC(D11)/10</f>
+        <v>518.5</v>
+      </c>
+      <c r="F11" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="G11" s="30" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="15.75" thickBot="1">
+      <c r="A12" s="17" t="s">
+        <v>87</v>
+      </c>
+      <c r="B12" s="45">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="C12" s="45">
+        <v>2</v>
+      </c>
+      <c r="D12" s="25" t="str">
+        <f t="shared" si="1"/>
+        <v>1551</v>
+      </c>
+      <c r="E12" s="25">
+        <f>HEX2DEC(D12)</f>
+        <v>5457</v>
+      </c>
+      <c r="F12" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="G12" s="26" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9">
+      <c r="A13" s="13" t="s">
+        <v>91</v>
+      </c>
+      <c r="B13" s="41">
+        <f t="shared" si="0"/>
+        <v>17</v>
+      </c>
+      <c r="C13" s="41">
+        <v>2</v>
+      </c>
+      <c r="D13" s="22" t="str">
+        <f t="shared" si="1"/>
+        <v>2112</v>
+      </c>
+      <c r="E13" s="22">
+        <f t="shared" ref="E13" si="2">HEX2DEC(D13)/10</f>
+        <v>846.6</v>
+      </c>
+      <c r="F13" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="G13" s="27" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9">
+      <c r="A14" s="18" t="s">
+        <v>92</v>
+      </c>
+      <c r="B14" s="46">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="C14" s="46">
+        <v>2</v>
+      </c>
+      <c r="D14" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v>2222</v>
+      </c>
+      <c r="E14" s="28">
+        <f t="shared" ref="E14" si="3">HEX2DEC(D14)/1000</f>
+        <v>8.7379999999999995</v>
+      </c>
+      <c r="F14" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="G14" s="29" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9">
+      <c r="A15" s="18" t="s">
+        <v>93</v>
+      </c>
+      <c r="B15" s="46">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="C15" s="46">
+        <v>2</v>
+      </c>
+      <c r="D15" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v>2332</v>
+      </c>
+      <c r="E15" s="28">
+        <f t="shared" ref="E15:E16" si="4">HEX2DEC(D15)/10</f>
+        <v>901</v>
+      </c>
+      <c r="F15" s="28" t="s">
+        <v>121</v>
+      </c>
+      <c r="G15" s="30" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9">
+      <c r="A16" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="B16" s="46">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="C16" s="46">
+        <v>2</v>
+      </c>
+      <c r="D16" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v>2442</v>
+      </c>
+      <c r="E16" s="28">
+        <f t="shared" si="4"/>
+        <v>928.2</v>
+      </c>
+      <c r="F16" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="G16" s="30" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A17" s="14" t="s">
+        <v>95</v>
+      </c>
+      <c r="B17" s="42">
+        <f t="shared" si="0"/>
+        <v>25</v>
+      </c>
+      <c r="C17" s="42">
+        <v>2</v>
+      </c>
+      <c r="D17" s="25" t="str">
+        <f t="shared" si="1"/>
+        <v>2552</v>
+      </c>
+      <c r="E17" s="25">
+        <f>HEX2DEC(D17)</f>
+        <v>9554</v>
+      </c>
+      <c r="F17" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="G17" s="26" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18" s="15" t="s">
+        <v>98</v>
+      </c>
+      <c r="B18" s="43">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="C18" s="43">
+        <v>2</v>
+      </c>
+      <c r="D18" s="22" t="str">
+        <f t="shared" si="1"/>
+        <v>3113</v>
+      </c>
+      <c r="E18" s="22">
+        <f t="shared" ref="E18" si="5">HEX2DEC(D18)/10</f>
+        <v>1256.3</v>
+      </c>
+      <c r="F18" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="G18" s="27" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19" s="16" t="s">
+        <v>99</v>
+      </c>
+      <c r="B19" s="44">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="C19" s="44">
+        <v>2</v>
+      </c>
+      <c r="D19" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v>3223</v>
+      </c>
+      <c r="E19" s="28">
+        <f t="shared" ref="E19" si="6">HEX2DEC(D19)/1000</f>
+        <v>12.835000000000001</v>
+      </c>
+      <c r="F19" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="G19" s="29" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="B20" s="44">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="C20" s="44">
+        <v>2</v>
+      </c>
+      <c r="D20" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v>3333</v>
+      </c>
+      <c r="E20" s="28">
+        <f t="shared" ref="E20:E21" si="7">HEX2DEC(D20)/10</f>
+        <v>1310.7</v>
+      </c>
+      <c r="F20" s="28" t="s">
+        <v>121</v>
+      </c>
+      <c r="G20" s="30" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="B21" s="44">
+        <f t="shared" si="0"/>
+        <v>33</v>
+      </c>
+      <c r="C21" s="44">
+        <v>2</v>
+      </c>
+      <c r="D21" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v>3443</v>
+      </c>
+      <c r="E21" s="28">
+        <f t="shared" si="7"/>
+        <v>1337.9</v>
+      </c>
+      <c r="F21" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="G21" s="30" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A22" s="17" t="s">
+        <v>102</v>
+      </c>
+      <c r="B22" s="45">
+        <f t="shared" si="0"/>
+        <v>35</v>
+      </c>
+      <c r="C22" s="45">
+        <v>2</v>
+      </c>
+      <c r="D22" s="25" t="str">
+        <f t="shared" si="1"/>
+        <v>3553</v>
+      </c>
+      <c r="E22" s="25">
+        <f>HEX2DEC(D22)</f>
+        <v>13651</v>
+      </c>
+      <c r="F22" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="G22" s="26" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="B23" s="41">
+        <f t="shared" si="0"/>
+        <v>37</v>
+      </c>
+      <c r="C23" s="41">
+        <v>2</v>
+      </c>
+      <c r="D23" s="22" t="str">
+        <f t="shared" si="1"/>
+        <v>4114</v>
+      </c>
+      <c r="E23" s="22">
+        <f t="shared" ref="E23" si="8">HEX2DEC(D23)/10</f>
+        <v>1666</v>
+      </c>
+      <c r="F23" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="G23" s="58" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24" s="18" t="s">
+        <v>104</v>
+      </c>
+      <c r="B24" s="46">
+        <f t="shared" si="0"/>
+        <v>39</v>
+      </c>
+      <c r="C24" s="46">
+        <v>2</v>
+      </c>
+      <c r="D24" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v>4224</v>
+      </c>
+      <c r="E24" s="28">
+        <f t="shared" ref="E24" si="9">HEX2DEC(D24)/1000</f>
+        <v>16.931999999999999</v>
+      </c>
+      <c r="F24" s="28" t="s">
+        <v>21</v>
+      </c>
+      <c r="G24" s="29" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25" s="18" t="s">
+        <v>105</v>
+      </c>
+      <c r="B25" s="46">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="C25" s="46">
+        <v>2</v>
+      </c>
+      <c r="D25" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v>4334</v>
+      </c>
+      <c r="E25" s="28">
+        <f t="shared" ref="E25:E26" si="10">HEX2DEC(D25)/10</f>
+        <v>1720.4</v>
+      </c>
+      <c r="F25" s="28" t="s">
+        <v>121</v>
+      </c>
+      <c r="G25" s="30" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="18" t="s">
+        <v>106</v>
+      </c>
+      <c r="B26" s="46">
+        <f t="shared" si="0"/>
+        <v>43</v>
+      </c>
+      <c r="C26" s="46">
+        <v>2</v>
+      </c>
+      <c r="D26" s="28" t="str">
+        <f t="shared" si="1"/>
+        <v>4444</v>
+      </c>
+      <c r="E26" s="28">
+        <f t="shared" si="10"/>
+        <v>1747.6</v>
+      </c>
+      <c r="F26" s="28" t="s">
+        <v>122</v>
+      </c>
+      <c r="G26" s="30" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" ht="15.75" thickBot="1">
+      <c r="A27" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="B27" s="42">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="C27" s="42">
+        <v>2</v>
+      </c>
+      <c r="D27" s="25" t="str">
+        <f t="shared" si="1"/>
+        <v>4554</v>
+      </c>
+      <c r="E27" s="25">
+        <f>HEX2DEC(D27)</f>
+        <v>17748</v>
+      </c>
+      <c r="F27" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="G27" s="26" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D1:H1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -2828,8 +3686,8 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>

<commit_message>
Quitada simulacion de datos de sensores en rutina de envio
</commit_message>
<xml_diff>
--- a/docs/Trama.xlsx
+++ b/docs/Trama.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Users\ProMatix\Dropbox\TAREAS\secretaria\est_monit_rio_jachal\Software Datalogger\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7B62516-D7E0-423C-A733-F52F6590B761}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B2CCC94-48EF-45B4-A782-2F16EA05AA16}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Reportes" sheetId="3" r:id="rId1"/>
@@ -1364,8 +1364,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:M69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="G61" sqref="G61"/>
+    <sheetView topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="D68" sqref="D68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2237,7 +2237,7 @@
   <dimension ref="A1:G26"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection sqref="A1:XFD1048576"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2717,8 +2717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B8ABDE8-E1B6-48E7-9A10-E5E726EB722B}">
   <dimension ref="A1:I27"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G23" sqref="G23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -3396,7 +3396,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>

</xml_diff>